<commit_message>
Revision 2 Mar 2023
</commit_message>
<xml_diff>
--- a/figures/ksTest/KS_test_pVals.xlsx
+++ b/figures/ksTest/KS_test_pVals.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20391"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\coskun-lab\Mythreye\SpatialOrganelles\20July2022 GitHub Revision 1\figures\ksTest\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BABD5C-71DE-4A41-AD7E-66746950B754}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="3">
   <si>
     <t>BM</t>
   </si>
@@ -28,20 +22,14 @@
     <t>UC</t>
   </si>
   <si>
-    <t>TOM20 vs HSP60</t>
-  </si>
-  <si>
-    <t>GOLPH4 vs Sortilin</t>
-  </si>
-  <si>
-    <t>Cell</t>
+    <t>inf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,32 +81,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -165,7 +138,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -197,27 +170,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -249,24 +204,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -442,169 +379,147 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>105.3090504242415</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>192.0926969490461</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>229.5949148951157</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>287.0503315615107</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4">
-        <v>4.9085088205908324E-106</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>8.0779851592192129E-193</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>2.5414706864969469E-230</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4">
-        <v>8.9057077352827538E-288</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>29.44233364222605</v>
+      </c>
+      <c r="C5">
+        <v>20.96678265014897</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4">
-        <v>3.611323198888011E-30</v>
-      </c>
-      <c r="C6" s="4">
-        <v>1.0794868340913459E-21</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>66.97990343472914</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1.0473614027117439E-67</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>189.887713506399</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1.2950498729108479E-190</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
-        <v>4.4114518122679048E-91</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
+      <c r="B8">
+        <v>90.35541846035211</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A1:A2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>